<commit_message>
Start to workmon full model. * Working on creating datasets
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -143,7 +143,7 @@
     <t xml:space="preserve">CA1 Interneuron Specific O-Targeting QuadD</t>
   </si>
   <si>
-    <t xml:space="preserve">CA1 Oriens/Alveus</t>
+    <t xml:space="preserve">CA1 Oriens-Alveus</t>
   </si>
   <si>
     <t xml:space="preserve">CA1 Oriens-Bistratified</t>
@@ -806,10 +806,10 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B13" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Work on model of net
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -221,7 +221,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -243,13 +242,11 @@
       <color rgb="FFCC0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -294,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,6 +309,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -320,7 +321,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -395,114 +396,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -512,7 +407,7 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.37"/>
   </cols>
@@ -800,1003 +695,1003 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B13" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="topRight" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="41.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="n">
+      <c r="B2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>160000</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="6" t="n">
         <v>2200</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="n">
+      <c r="B3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="n">
         <v>312</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="5" t="n">
         <f aca="false">ROUND(D3/10,0)*B3</f>
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="4" t="n">
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="5" t="n">
         <v>29</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="n">
+      <c r="B4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>203</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="5" t="n">
         <f aca="false">ROUND(D4/10,0)*B4</f>
         <v>20</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="n">
+      <c r="B5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="n">
         <v>793</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <f aca="false">ROUND(D5/10,0)*B5</f>
         <v>79</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="5"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="n">
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="n">
         <v>336</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <f aca="false">ROUND(D6/10,0)*B6</f>
         <v>34</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="n">
+      <c r="B7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="n">
         <v>333</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="5" t="n">
         <f aca="false">ROUND(D7/10,0)*B7</f>
         <v>33</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="n">
+      <c r="B8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="n">
         <v>395</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <f aca="false">ROUND(D8/10,0)*B8</f>
         <v>40</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="n">
+      <c r="B9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="n">
         <v>804</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="5" t="n">
         <f aca="false">ROUND(D9/10,0)*B9</f>
         <v>80</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="4" t="n">
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="n">
         <v>27</v>
       </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="n">
+      <c r="B10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="n">
         <v>118</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="5" t="n">
         <f aca="false">ROUND(D10/10,0)*B10</f>
         <v>0</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="n">
+      <c r="B11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="n">
         <v>778</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="5" t="n">
         <f aca="false">ROUND(D11/10,0)*B11</f>
         <v>78</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4" t="n">
+      <c r="B12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>837</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="5" t="n">
         <f aca="false">ROUND(D12/10,0)*B12</f>
         <v>84</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4" t="n">
+      <c r="B13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>171</v>
       </c>
-      <c r="E13" s="4" t="n">
+      <c r="E13" s="5" t="n">
         <f aca="false">ROUND(D13/10,0)*B13</f>
         <v>17</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4" t="n">
+      <c r="B14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="E14" s="5" t="n">
         <f aca="false">ROUND(D14/10,0)*B14</f>
         <v>14</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4" t="n">
+      <c r="B15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>1010</v>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="5" t="n">
         <f aca="false">ROUND(D15/10,0)*B15</f>
         <v>101</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="n">
+      <c r="B16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5" t="n">
         <v>658</v>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="5" t="n">
         <f aca="false">ROUND(D16/10,0)*B16</f>
         <v>66</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="5"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="n">
+      <c r="B17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="n">
         <v>1114</v>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="E17" s="5" t="n">
         <f aca="false">ROUND(D17/10,0)*B17</f>
         <v>111</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="4" t="s">
+      <c r="G17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="n">
+      <c r="B18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="n">
         <v>96</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="5" t="n">
         <f aca="false">ROUND(D18/10,0)*B18</f>
         <v>10</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4" t="n">
+      <c r="B19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="n">
         <v>521</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="5" t="n">
         <f aca="false">ROUND(D19/10,0)*B19</f>
         <v>52</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="G19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="n">
+      <c r="B20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="5" t="n">
         <f aca="false">ROUND(D20/10,0)*B20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4" t="n">
+      <c r="B21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="n">
         <v>574</v>
       </c>
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="5" t="n">
         <f aca="false">ROUND(D21/10,0)*B21</f>
         <v>57</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="5"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4" t="n">
+      <c r="B22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5" t="n">
         <v>73</v>
       </c>
-      <c r="E22" s="4" t="n">
+      <c r="E22" s="5" t="n">
         <f aca="false">ROUND(D22/10,0)*B22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="5"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4" t="n">
+      <c r="B23" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5" t="n">
         <v>171</v>
       </c>
-      <c r="E23" s="4" t="n">
+      <c r="E23" s="5" t="n">
         <f aca="false">ROUND(D23/10,0)*B23</f>
         <v>17</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="n">
+      <c r="B24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="n">
         <v>607</v>
       </c>
-      <c r="E24" s="4" t="n">
+      <c r="E24" s="5" t="n">
         <f aca="false">ROUND(D24/10,0)*B24</f>
         <v>61</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="5"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4" t="n">
+      <c r="B25" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="n">
         <v>340</v>
       </c>
-      <c r="E25" s="4" t="n">
+      <c r="E25" s="5" t="n">
         <f aca="false">ROUND(D25/10,0)*B25</f>
         <v>34</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="5"/>
       <c r="I25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="4" t="n">
+      <c r="B26" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5" t="n">
         <v>191</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="5" t="n">
         <f aca="false">ROUND(D26/10,0)*B26</f>
         <v>19</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="4"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4" t="n">
+      <c r="B27" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="n">
         <v>729</v>
       </c>
-      <c r="E27" s="4" t="n">
+      <c r="E27" s="5" t="n">
         <f aca="false">ROUND(D27/10,0)*B27</f>
         <v>73</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="4"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4" t="n">
+      <c r="B28" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="n">
         <v>463</v>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="E28" s="5" t="n">
         <f aca="false">ROUND(D28/10,0)*B28</f>
         <v>46</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="4" t="s">
+      <c r="G28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>46</v>
       </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="4" t="n">
+      <c r="B29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="E29" s="4" t="n">
+      <c r="E29" s="5" t="n">
         <f aca="false">ROUND(D29/10,0)*B29</f>
         <v>0</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4" t="n">
+      <c r="B30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E30" s="4" t="n">
+      <c r="E30" s="5" t="n">
         <f aca="false">ROUND(D30/10,0)*B30</f>
         <v>0</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4" t="n">
+      <c r="B31" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5" t="n">
         <v>698</v>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="5" t="n">
         <f aca="false">ROUND(D31/10,0)*B31</f>
         <v>70</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="4" t="s">
+      <c r="G31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4" t="n">
+      <c r="B32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="n">
         <v>128</v>
       </c>
-      <c r="E32" s="4" t="n">
+      <c r="E32" s="5" t="n">
         <f aca="false">ROUND(D32/10,0)*B32</f>
         <v>13</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="5"/>
       <c r="I32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4" t="n">
+      <c r="B33" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="E33" s="4" t="n">
+      <c r="E33" s="5" t="n">
         <f aca="false">ROUND(D33/10,0)*B33</f>
         <v>9</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="4"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="5"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="4" t="n">
+      <c r="B34" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5" t="n">
         <v>171</v>
       </c>
-      <c r="E34" s="4" t="n">
+      <c r="E34" s="5" t="n">
         <f aca="false">ROUND(D34/10,0)*B34</f>
         <v>17</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="4" t="s">
+      <c r="G34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I34" s="3"/>
     </row>
     <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="4" t="n">
+      <c r="B35" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="n">
         <v>986</v>
       </c>
-      <c r="E35" s="4" t="n">
+      <c r="E35" s="5" t="n">
         <f aca="false">ROUND(D35/10,0)*B35</f>
         <v>99</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="4"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="5"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4" t="n">
+      <c r="B36" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5" t="n">
         <v>84</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="5" t="n">
         <f aca="false">ROUND(D36/10,0)*B36</f>
         <v>8</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="4"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4" t="n">
+      <c r="B37" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="n">
         <v>313</v>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="E37" s="5" t="n">
         <f aca="false">ROUND(D37/10,0)*B37</f>
         <v>31</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="4"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="5"/>
       <c r="I37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4" t="n">
+      <c r="B38" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="n">
         <v>401</v>
       </c>
-      <c r="E38" s="4" t="n">
+      <c r="E38" s="5" t="n">
         <f aca="false">ROUND(D38/10,0)*B38</f>
         <v>40</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="4" t="s">
+      <c r="G38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>60</v>
       </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4" t="n">
+      <c r="B39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="n">
         <v>119</v>
       </c>
-      <c r="E39" s="4" t="n">
+      <c r="E39" s="5" t="n">
         <f aca="false">ROUND(D39/10,0)*B39</f>
         <v>0</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="4"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="5"/>
       <c r="I39" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on fit network only theta rhythm
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="local_model" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="theta_model" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="75">
   <si>
     <t xml:space="preserve">neurons</t>
   </si>
@@ -207,6 +208,45 @@
   </si>
   <si>
     <t xml:space="preserve">CA1 Radial Trilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutPlaceThetaPhase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutPlaceFiringRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InPlacePeakRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CenterPlaceField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SigmaPlaceField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SlopePhasePrecession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrecessionOnset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA3_generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEC_generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5</t>
   </si>
 </sst>
 </file>
@@ -287,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,6 +354,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -441,7 +485,7 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2455,4 +2499,1499 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="41.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="7" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K2" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L2" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L3" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>312</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <f aca="false">ROUND(D4*0.0025,0)*B4</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>203</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K5" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L5" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>793</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K6" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>336</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <f aca="false">ROUND(D7*0.0025,0)*B7</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>333</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>395</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <f aca="false">ROUND(D9*0.0025,0)*B9</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>804</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <f aca="false">ROUND(D11*0.0025,0)*B11</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K11" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>778</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L12" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>837</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K13" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L13" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <f aca="false">ROUND(D14*0.0025,0)*B14</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J14" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K14" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>136</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <f aca="false">ROUND(D15*0.0025,0)*B15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K15" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L15" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>1010</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J16" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K16" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>658</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J17" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K17" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L17" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>1114</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J18" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K18" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L18" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <f aca="false">ROUND(D19*0.0025,0)*B19</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J19" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K19" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L19" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>521</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <f aca="false">ROUND(D20*0.0025,0)*B20</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J20" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K20" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L20" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <f aca="false">ROUND(D21*0.0025,0)*B21</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J21" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K21" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L21" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>574</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <f aca="false">ROUND(D22*0.0025,0)*B22</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J22" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K22" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L22" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <f aca="false">ROUND(D23*0.0025,0)*B23</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J23" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K23" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L23" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <f aca="false">ROUND(D24*0.0025,0)*B24</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J24" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K24" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L24" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>607</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J25" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K25" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L25" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>340</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J26" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K26" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L26" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>191</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <f aca="false">ROUND(D27*0.0025,0)*B27</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J27" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K27" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L27" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>729</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J28" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K28" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L28" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>463</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <f aca="false">ROUND(D29*0.0025,0)*B29</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J29" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K29" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L29" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <f aca="false">ROUND(D30*0.0025,0)*B30</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J30" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K30" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L30" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <f aca="false">ROUND(D31*0.0025,0)*B31</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J31" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K31" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L31" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>698</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J32" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K32" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L32" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>128</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <f aca="false">ROUND(D33*0.0025,0)*B33</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J33" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K33" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L33" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <f aca="false">ROUND(D34*0.0025,0)*B34</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J34" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K34" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L34" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J35" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K35" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L35" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>986</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J36" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K36" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L36" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <f aca="false">ROUND(D37*0.0025,0)*B37</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J37" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K37" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L37" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>313</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J38" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K38" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L38" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>401</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <f aca="false">ROUND(D39*0.0025,0)*B39</f>
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I39" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J39" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K39" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L39" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <f aca="false">ROUND(D40*0.0025,0)*B40</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J40" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K40" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L40" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J41" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K41" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L41" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J42" s="7" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K42" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L42" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add MEC 3 to CA1 Trilaminar connection
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -327,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,10 +354,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2508,8 +2504,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2522,7 +2518,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="7" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,16 +2549,16 @@
       <c r="I1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2594,13 +2590,13 @@
       <c r="I2" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K2" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L2" s="7" t="n">
+      <c r="J2" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2632,13 +2628,13 @@
       <c r="I3" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K3" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L3" s="7" t="n">
+      <c r="J3" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L3" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2671,13 +2667,13 @@
       <c r="I4" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J4" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K4" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L4" s="7" t="n">
+      <c r="J4" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2703,13 +2699,13 @@
       <c r="I5" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J5" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K5" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L5" s="7" t="n">
+      <c r="J5" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L5" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2735,13 +2731,13 @@
       <c r="I6" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J6" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K6" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L6" s="7" t="n">
+      <c r="J6" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2774,13 +2770,13 @@
       <c r="I7" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J7" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K7" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L7" s="7" t="n">
+      <c r="J7" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2806,13 +2802,13 @@
       <c r="I8" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J8" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K8" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L8" s="7" t="n">
+      <c r="J8" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L8" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2845,13 +2841,13 @@
       <c r="I9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J9" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K9" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L9" s="7" t="n">
+      <c r="J9" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2883,13 +2879,13 @@
       <c r="I10" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J10" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K10" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L10" s="7" t="n">
+      <c r="J10" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2916,13 +2912,13 @@
       <c r="I11" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J11" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K11" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L11" s="7" t="n">
+      <c r="J11" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2954,13 +2950,13 @@
       <c r="I12" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J12" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K12" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L12" s="7" t="n">
+      <c r="J12" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L12" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2986,13 +2982,13 @@
       <c r="I13" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J13" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K13" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L13" s="7" t="n">
+      <c r="J13" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L13" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3019,13 +3015,13 @@
       <c r="I14" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J14" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K14" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L14" s="7" t="n">
+      <c r="J14" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K14" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L14" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3052,13 +3048,13 @@
       <c r="I15" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J15" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K15" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L15" s="7" t="n">
+      <c r="J15" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L15" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3084,13 +3080,13 @@
       <c r="I16" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J16" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K16" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L16" s="7" t="n">
+      <c r="J16" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3116,13 +3112,13 @@
       <c r="I17" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J17" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K17" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L17" s="7" t="n">
+      <c r="J17" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L17" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3154,13 +3150,13 @@
       <c r="I18" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J18" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K18" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L18" s="7" t="n">
+      <c r="J18" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L18" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3187,13 +3183,13 @@
       <c r="I19" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J19" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K19" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L19" s="7" t="n">
+      <c r="J19" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L19" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3226,13 +3222,13 @@
       <c r="I20" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J20" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K20" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L20" s="7" t="n">
+      <c r="J20" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L20" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3259,13 +3255,13 @@
       <c r="I21" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J21" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K21" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L21" s="7" t="n">
+      <c r="J21" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L21" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3291,13 +3287,13 @@
       <c r="I22" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J22" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K22" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L22" s="7" t="n">
+      <c r="J22" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K22" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L22" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3324,13 +3320,13 @@
       <c r="I23" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J23" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K23" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L23" s="7" t="n">
+      <c r="J23" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K23" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L23" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3357,13 +3353,13 @@
       <c r="I24" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J24" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K24" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L24" s="7" t="n">
+      <c r="J24" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K24" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L24" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3389,13 +3385,13 @@
       <c r="I25" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J25" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K25" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L25" s="7" t="n">
+      <c r="J25" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L25" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3421,13 +3417,13 @@
       <c r="I26" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J26" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K26" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L26" s="7" t="n">
+      <c r="J26" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L26" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3454,13 +3450,13 @@
       <c r="I27" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J27" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K27" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L27" s="7" t="n">
+      <c r="J27" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L27" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3486,13 +3482,13 @@
       <c r="I28" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J28" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K28" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L28" s="7" t="n">
+      <c r="J28" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L28" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3525,13 +3521,13 @@
       <c r="I29" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J29" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K29" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L29" s="7" t="n">
+      <c r="J29" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K29" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L29" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3558,13 +3554,13 @@
       <c r="I30" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J30" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K30" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L30" s="7" t="n">
+      <c r="J30" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K30" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L30" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3591,13 +3587,13 @@
       <c r="I31" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J31" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K31" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L31" s="7" t="n">
+      <c r="J31" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K31" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L31" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3629,13 +3625,13 @@
       <c r="I32" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J32" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K32" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L32" s="7" t="n">
+      <c r="J32" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K32" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L32" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3662,13 +3658,13 @@
       <c r="I33" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J33" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K33" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L33" s="7" t="n">
+      <c r="J33" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L33" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3695,13 +3691,13 @@
       <c r="I34" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J34" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K34" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L34" s="7" t="n">
+      <c r="J34" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L34" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3733,13 +3729,13 @@
       <c r="I35" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J35" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K35" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L35" s="7" t="n">
+      <c r="J35" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L35" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3765,13 +3761,13 @@
       <c r="I36" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J36" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K36" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L36" s="7" t="n">
+      <c r="J36" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K36" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L36" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3798,13 +3794,13 @@
       <c r="I37" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J37" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K37" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L37" s="7" t="n">
+      <c r="J37" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K37" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L37" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3830,13 +3826,13 @@
       <c r="I38" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J38" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K38" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L38" s="7" t="n">
+      <c r="J38" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K38" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L38" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3869,13 +3865,13 @@
       <c r="I39" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J39" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K39" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L39" s="7" t="n">
+      <c r="J39" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L39" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3902,13 +3898,13 @@
       <c r="I40" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J40" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K40" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L40" s="7" t="n">
+      <c r="J40" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L40" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3940,13 +3936,13 @@
       <c r="I41" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J41" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K41" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L41" s="7" t="n">
+      <c r="J41" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L41" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3978,13 +3974,13 @@
       <c r="I42" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J42" s="7" t="n">
-        <v>-100000</v>
-      </c>
-      <c r="K42" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="L42" s="7" t="n">
+      <c r="J42" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="K42" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="L42" s="3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work on numpy class for mean field integration
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="78">
   <si>
     <t xml:space="preserve">neurons</t>
   </si>
@@ -231,10 +231,16 @@
     <t xml:space="preserve">PrecessionOnset</t>
   </si>
   <si>
+    <t xml:space="preserve">CA1 Pyramidal (deep)</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.25</t>
   </si>
   <si>
     <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA1 Pyramidal (superficial)</t>
   </si>
   <si>
     <t xml:space="preserve">8.5</t>
@@ -259,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -286,6 +292,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +368,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2507,8 +2522,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2566,8 +2581,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
+      <c r="A2" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
@@ -2585,10 +2600,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>8</v>
@@ -2604,8 +2619,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
+      <c r="A3" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1</v>
@@ -2623,10 +2638,10 @@
         <v>22</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>8</v>
@@ -3863,7 +3878,7 @@
         <v>11</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I39" s="3" t="n">
         <v>8</v>
@@ -3913,7 +3928,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B41" s="3" t="n">
         <v>1</v>
@@ -3928,13 +3943,13 @@
         <v>1</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I41" s="3" t="n">
         <v>8</v>
@@ -3951,7 +3966,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B42" s="3" t="n">
         <v>1</v>
@@ -3969,10 +3984,10 @@
         <v>50</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I42" s="3" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
Work with trilaminar cells
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -265,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -292,11 +292,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -341,7 +336,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,10 +363,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2522,8 +2513,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2581,7 +2572,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="4" t="n">
@@ -2619,7 +2610,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -3872,10 +3863,10 @@
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Work on theta verification
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="local_model" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="theta_model" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="verified_theta_model" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="126">
   <si>
     <t xml:space="preserve">neurons</t>
   </si>
@@ -259,6 +260,147 @@
   </si>
   <si>
     <t xml:space="preserve">1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hippocampome_Neurons_Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model_Neurons_Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyramidal (deep)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyramidal (superficial)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axo-Axonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Axo-Axonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back-Projection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basket CCK+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bistratified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hippocampo-subicular Projecting ENK+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific LM-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific LMO-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific LMR-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMR Projecting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neurogliaform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neurogliaform Projecting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O-LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurrent O-LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O-LMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific O-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific O-Targeting QuadD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oriens-Alveus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oriens-Bistratified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oriens-Bistratified Projecting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OR-LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perforant Path-Associated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perforant Path-Associated QuadD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quadrilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interneuron Specific R-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-Receiving Apical-Targeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific RO-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schaffer Collateral-Associated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SO-SO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radial Trilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA3 Pyramidal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA3 Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EC LIII Pyramidal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEC Input</t>
   </si>
 </sst>
 </file>
@@ -268,7 +410,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -295,6 +437,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -339,7 +486,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,6 +513,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -493,7 +644,7 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1505,7 +1656,7 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -2516,8 +2667,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4005,4 +4156,1756 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="41.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="26.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="21.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="15.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="3" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="12" style="3" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>312</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">ROUND(F4*0.0025,0)*D4</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>203</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>793</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>336</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">ROUND(F7*0.0025,0)*D7</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>333</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>395</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <f aca="false">ROUND(F9*0.0025,0)*D9</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M9" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>804</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <f aca="false">ROUND(F11*0.0025,0)*D11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>778</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>837</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L13" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M13" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <f aca="false">ROUND(F14*0.0025,0)*D14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M14" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>136</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <f aca="false">ROUND(F15*0.0025,0)*D15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M15" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>1010</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L16" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M16" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N16" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>658</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L17" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M17" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N17" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>1114</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M18" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">ROUND(F19*0.0025,0)*D19</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M19" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>521</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <f aca="false">ROUND(F20*0.0025,0)*D20</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L20" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M20" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N20" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <f aca="false">ROUND(F21*0.0025,0)*D21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M21" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N21" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>574</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M22" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N22" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <f aca="false">ROUND(F23*0.0025,0)*D23</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L23" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M23" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N23" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <f aca="false">ROUND(F24*0.0025,0)*D24</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L24" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M24" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N24" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>607</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M25" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N25" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>340</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L26" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M26" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N26" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>191</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <f aca="false">ROUND(F27*0.0025,0)*D27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L27" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M27" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N27" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>729</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M28" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>463</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <f aca="false">ROUND(F29*0.0025,0)*D29</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K29" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M29" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N29" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <f aca="false">ROUND(F30*0.0025,0)*D30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L30" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M30" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N30" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <f aca="false">ROUND(F31*0.0025,0)*D31</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L31" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M31" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N31" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>698</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K32" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M32" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N32" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>128</v>
+      </c>
+      <c r="G33" s="3" t="n">
+        <f aca="false">ROUND(F33*0.0025,0)*D33</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L33" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M33" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N33" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="G34" s="3" t="n">
+        <f aca="false">ROUND(F34*0.0025,0)*D34</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M34" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N34" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="G35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M35" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N35" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>986</v>
+      </c>
+      <c r="G36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M36" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N36" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <f aca="false">ROUND(F37*0.0025,0)*D37</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L37" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M37" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N37" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>313</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L38" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M38" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N38" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>401</v>
+      </c>
+      <c r="G39" s="3" t="n">
+        <f aca="false">ROUND(F39*0.0025,0)*D39</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L39" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M39" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N39" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <f aca="false">ROUND(F40*0.0025,0)*D40</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L40" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M40" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N40" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M41" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N41" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K42" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L42" s="3" t="n">
+        <v>-100000</v>
+      </c>
+      <c r="M42" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="N42" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work on R optimization
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -410,7 +410,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -437,11 +437,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -486,7 +481,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,10 +508,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -644,7 +635,7 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1656,9 +1647,9 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B25" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
       <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2667,8 +2658,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4165,8 +4156,8 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4188,7 +4179,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -5751,7 +5742,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Pyramidal neurons are generators. Git resetted to augoust variant
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -274,15 +274,18 @@
     <t xml:space="preserve">Pyramidal (deep)</t>
   </si>
   <si>
+    <t xml:space="preserve">generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyramidal (superficial)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axo-Axonic</t>
+  </si>
+  <si>
     <t xml:space="preserve">simulated</t>
   </si>
   <si>
-    <t xml:space="preserve">Pyramidal (superficial)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Axo-Axonic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Horizontal Axo-Axonic</t>
   </si>
   <si>
@@ -392,9 +395,6 @@
   </si>
   <si>
     <t xml:space="preserve">CA3 Input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generator</t>
   </si>
   <si>
     <t xml:space="preserve">EC LIII Pyramidal</t>
@@ -4166,7 +4166,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4238,7 +4238,7 @@
       <c r="B2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="4" t="n">
@@ -4282,7 +4282,7 @@
       <c r="B3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D3" s="4" t="n">
@@ -4327,7 +4327,7 @@
         <v>85</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>1</v>
@@ -4369,10 +4369,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>1</v>
@@ -4407,10 +4407,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>1</v>
@@ -4445,10 +4445,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>1</v>
@@ -4490,10 +4490,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>1</v>
@@ -4528,10 +4528,10 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>1</v>
@@ -4573,10 +4573,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>1</v>
@@ -4617,10 +4617,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>0</v>
@@ -4656,10 +4656,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>1</v>
@@ -4700,10 +4700,10 @@
         <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>1</v>
@@ -4738,10 +4738,10 @@
         <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>1</v>
@@ -4777,10 +4777,10 @@
         <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>1</v>
@@ -4816,10 +4816,10 @@
         <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D16" s="3" t="n">
         <v>1</v>
@@ -4854,10 +4854,10 @@
         <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>1</v>
@@ -4892,10 +4892,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D18" s="3" t="n">
         <v>1</v>
@@ -4936,10 +4936,10 @@
         <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D19" s="3" t="n">
         <v>1</v>
@@ -4975,10 +4975,10 @@
         <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>1</v>
@@ -5020,10 +5020,10 @@
         <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>0</v>
@@ -5059,10 +5059,10 @@
         <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>1</v>
@@ -5097,10 +5097,10 @@
         <v>38</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>0</v>
@@ -5136,10 +5136,10 @@
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>1</v>
@@ -5175,10 +5175,10 @@
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>1</v>
@@ -5213,10 +5213,10 @@
         <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>1</v>
@@ -5251,10 +5251,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>1</v>
@@ -5290,10 +5290,10 @@
         <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>1</v>
@@ -5327,11 +5327,11 @@
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>110</v>
+      <c r="B29" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>1</v>
@@ -5373,10 +5373,10 @@
         <v>47</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D30" s="3" t="n">
         <v>0</v>
@@ -5412,10 +5412,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D31" s="3" t="n">
         <v>0</v>
@@ -5451,10 +5451,10 @@
         <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D32" s="3" t="n">
         <v>1</v>
@@ -5495,10 +5495,10 @@
         <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D33" s="3" t="n">
         <v>1</v>
@@ -5534,10 +5534,10 @@
         <v>53</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D34" s="3" t="n">
         <v>1</v>
@@ -5573,10 +5573,10 @@
         <v>54</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D35" s="3" t="n">
         <v>1</v>
@@ -5617,10 +5617,10 @@
         <v>55</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>1</v>
@@ -5658,7 +5658,7 @@
         <v>56</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D37" s="3" t="n">
         <v>1</v>
@@ -5694,10 +5694,10 @@
         <v>57</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D38" s="3" t="n">
         <v>1</v>
@@ -5732,10 +5732,10 @@
         <v>58</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D39" s="3" t="n">
         <v>1</v>
@@ -5777,10 +5777,10 @@
         <v>61</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="n">
         <v>0</v>
@@ -5813,13 +5813,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="D41" s="3" t="n">
         <v>1</v>
@@ -5863,7 +5863,7 @@
         <v>125</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="D42" s="3" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Pyramidal neurons are generators. Git resetted to augoust variant New branch
</commit_message>
<xml_diff>
--- a/parameters/neurons_parameters.xlsx
+++ b/parameters/neurons_parameters.xlsx
@@ -271,136 +271,136 @@
     <t xml:space="preserve">Simulated_Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Axo-Axonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Axo-Axonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back-Projection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal Basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basket CCK+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bistratified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hippocampo-subicular Projecting ENK+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific LM-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific LMO-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific LMR-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMR Projecting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neurogliaform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neurogliaform Projecting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O-LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurrent O-LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O-LMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific O-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific O-Targeting QuadD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oriens-Alveus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oriens-Bistratified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oriens-Bistratified Projecting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OR-LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perforant Path-Associated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perforant Path-Associated QuadD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quadrilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific R-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-Receiving Apical-Targeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interneuron Specific RO-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schaffer Collateral-Associated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SO-SO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radial Trilaminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA3 Pyramidal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA3 Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EC LIII Pyramidal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEC Input</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pyramidal (deep)</t>
   </si>
   <si>
-    <t xml:space="preserve">simulated</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pyramidal (superficial)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Axo-Axonic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horizontal Axo-Axonic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Back-Projection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horizontal Basket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basket CCK+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bistratified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hippocampo-subicular Projecting ENK+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific LM-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific LMO-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific LMR-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMR Projecting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neurogliaform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neurogliaform Projecting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O-LM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recurrent O-LM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O-LMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific O-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific O-Targeting QuadD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oriens-Alveus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oriens-Bistratified</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oriens-Bistratified Projecting</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OR-LM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perforant Path-Associated</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Perforant Path-Associated QuadD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quadrilaminar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific R-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R-Receiving Apical-Targeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radiatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interneuron Specific RO-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schaffer Collateral-Associated</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SO-SO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trilaminar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radial Trilaminar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA3 Pyramidal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA3 Input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EC LIII Pyramidal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEC Input</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -437,11 +437,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -486,7 +481,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,10 +508,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2297,7 +2288,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -2345,7 +2336,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>44</v>
       </c>
@@ -2473,7 +2464,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -2525,7 +2516,7 @@
       </c>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
         <v>55</v>
       </c>
@@ -4166,7 +4157,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4184,7 +4175,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="12" style="3" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -4232,35 +4223,36 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="n">
-        <v>160000</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="3" t="n">
+        <v>312</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <f aca="false">ROUND(F2*0.0025,0)*D2</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>71</v>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>29</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>8</v>
@@ -4276,35 +4268,29 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="n">
-        <v>160000</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>71</v>
+      <c r="F3" s="3" t="n">
+        <v>203</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="K3" s="3" t="n">
         <v>8</v>
@@ -4321,7 +4307,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>85</v>
@@ -4336,20 +4322,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>312</v>
+        <v>793</v>
       </c>
       <c r="G4" s="3" t="n">
-        <f aca="false">ROUND(F4*0.0025,0)*D4</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>29</v>
       </c>
       <c r="K4" s="3" t="n">
         <v>8</v>
@@ -4366,7 +4345,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>86</v>
@@ -4381,13 +4360,20 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>203</v>
+        <v>336</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>0</v>
+        <f aca="false">ROUND(F5*0.0025,0)*D5</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>8</v>
@@ -4404,7 +4390,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>87</v>
@@ -4419,7 +4405,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>793</v>
+        <v>333</v>
       </c>
       <c r="G6" s="3" t="n">
         <v>0</v>
@@ -4442,7 +4428,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>88</v>
@@ -4457,20 +4443,20 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>336</v>
+        <v>395</v>
       </c>
       <c r="G7" s="3" t="n">
         <f aca="false">ROUND(F7*0.0025,0)*D7</f>
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>8</v>
@@ -4487,7 +4473,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>89</v>
@@ -4502,13 +4488,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>333</v>
+        <v>804</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>27</v>
       </c>
       <c r="K8" s="3" t="n">
         <v>8</v>
@@ -4525,7 +4517,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>90</v>
@@ -4534,26 +4526,20 @@
         <v>83</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>395</v>
+        <v>118</v>
       </c>
       <c r="G9" s="3" t="n">
         <f aca="false">ROUND(F9*0.0025,0)*D9</f>
-        <v>1</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="K9" s="3" t="n">
         <v>8</v>
@@ -4570,7 +4556,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>91</v>
@@ -4585,19 +4571,19 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>804</v>
+        <v>778</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="3" t="n">
-        <v>27</v>
+      <c r="J10" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="K10" s="3" t="n">
         <v>8</v>
@@ -4614,7 +4600,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>92</v>
@@ -4623,16 +4609,15 @@
         <v>83</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>118</v>
+        <v>837</v>
       </c>
       <c r="G11" s="3" t="n">
-        <f aca="false">ROUND(F11*0.0025,0)*D11</f>
         <v>0</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -4653,7 +4638,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>93</v>
@@ -4665,22 +4650,17 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>778</v>
+        <v>171</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>19</v>
+        <f aca="false">ROUND(F12*0.0025,0)*D12</f>
+        <v>0</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="K12" s="3" t="n">
         <v>8</v>
@@ -4697,7 +4677,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>94</v>
@@ -4709,12 +4689,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>837</v>
+        <v>136</v>
       </c>
       <c r="G13" s="3" t="n">
+        <f aca="false">ROUND(F13*0.0025,0)*D13</f>
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
@@ -4735,7 +4716,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>95</v>
@@ -4750,10 +4731,9 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>171</v>
+        <v>1010</v>
       </c>
       <c r="G14" s="3" t="n">
-        <f aca="false">ROUND(F14*0.0025,0)*D14</f>
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -4774,7 +4754,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>96</v>
@@ -4786,13 +4766,12 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>136</v>
+        <v>658</v>
       </c>
       <c r="G15" s="3" t="n">
-        <f aca="false">ROUND(F15*0.0025,0)*D15</f>
         <v>0</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -4813,7 +4792,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>97</v>
@@ -4825,16 +4804,22 @@
         <v>1</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>1010</v>
+        <v>1114</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K16" s="3" t="n">
         <v>8</v>
@@ -4851,7 +4836,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>98</v>
@@ -4863,12 +4848,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>658</v>
+        <v>96</v>
       </c>
       <c r="G17" s="3" t="n">
+        <f aca="false">ROUND(F17*0.0025,0)*D17</f>
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -4889,7 +4875,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>99</v>
@@ -4904,19 +4890,20 @@
         <v>1</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>1114</v>
+        <v>521</v>
       </c>
       <c r="G18" s="3" t="n">
+        <f aca="false">ROUND(F18*0.0025,0)*D18</f>
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K18" s="3" t="n">
         <v>8</v>
@@ -4933,7 +4920,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>100</v>
@@ -4942,13 +4929,13 @@
         <v>83</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="G19" s="3" t="n">
         <f aca="false">ROUND(F19*0.0025,0)*D19</f>
@@ -4972,7 +4959,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>101</v>
@@ -4987,20 +4974,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>521</v>
+        <v>574</v>
       </c>
       <c r="G20" s="3" t="n">
-        <f aca="false">ROUND(F20*0.0025,0)*D20</f>
-        <v>1</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="K20" s="3" t="n">
         <v>8</v>
@@ -5017,7 +4997,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>102</v>
@@ -5029,10 +5009,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G21" s="3" t="n">
         <f aca="false">ROUND(F21*0.0025,0)*D21</f>
@@ -5056,7 +5036,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>103</v>
@@ -5068,12 +5048,13 @@
         <v>1</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>574</v>
+        <v>171</v>
       </c>
       <c r="G22" s="3" t="n">
+        <f aca="false">ROUND(F22*0.0025,0)*D22</f>
         <v>0</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -5094,7 +5075,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>104</v>
@@ -5103,16 +5084,15 @@
         <v>83</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>73</v>
+        <v>607</v>
       </c>
       <c r="G23" s="3" t="n">
-        <f aca="false">ROUND(F23*0.0025,0)*D23</f>
         <v>0</v>
       </c>
       <c r="I23" s="3" t="s">
@@ -5133,7 +5113,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>105</v>
@@ -5145,13 +5125,12 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>171</v>
+        <v>340</v>
       </c>
       <c r="G24" s="3" t="n">
-        <f aca="false">ROUND(F24*0.0025,0)*D24</f>
         <v>0</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -5172,7 +5151,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>106</v>
@@ -5184,12 +5163,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>607</v>
+        <v>191</v>
       </c>
       <c r="G25" s="3" t="n">
+        <f aca="false">ROUND(F25*0.0025,0)*D25</f>
         <v>0</v>
       </c>
       <c r="I25" s="3" t="s">
@@ -5210,7 +5190,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>107</v>
@@ -5225,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="3" t="n">
-        <v>340</v>
+        <v>729</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>0</v>
@@ -5247,10 +5227,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -5260,17 +5240,23 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="n">
-        <v>191</v>
+        <v>463</v>
       </c>
       <c r="G27" s="3" t="n">
         <f aca="false">ROUND(F27*0.0025,0)*D27</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="K27" s="3" t="n">
         <v>8</v>
@@ -5287,7 +5273,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>109</v>
@@ -5296,15 +5282,16 @@
         <v>83</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="3" t="n">
-        <v>729</v>
+        <v>22</v>
       </c>
       <c r="G28" s="3" t="n">
+        <f aca="false">ROUND(F28*0.0025,0)*D28</f>
         <v>0</v>
       </c>
       <c r="I28" s="3" t="s">
@@ -5324,36 +5311,30 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>110</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>463</v>
+        <v>9</v>
       </c>
       <c r="G29" s="3" t="n">
         <f aca="false">ROUND(F29*0.0025,0)*D29</f>
-        <v>1</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="K29" s="3" t="n">
         <v>8</v>
@@ -5370,7 +5351,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>111</v>
@@ -5379,20 +5360,25 @@
         <v>83</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3" t="n">
-        <v>22</v>
+        <v>698</v>
       </c>
       <c r="G30" s="3" t="n">
-        <f aca="false">ROUND(F30*0.0025,0)*D30</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="K30" s="3" t="n">
         <v>8</v>
@@ -5409,7 +5395,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>112</v>
@@ -5418,13 +5404,13 @@
         <v>83</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F31" s="3" t="n">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="G31" s="3" t="n">
         <f aca="false">ROUND(F31*0.0025,0)*D31</f>
@@ -5448,7 +5434,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>113</v>
@@ -5460,22 +5446,17 @@
         <v>1</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="3" t="n">
-        <v>698</v>
+        <v>93</v>
       </c>
       <c r="G32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>50</v>
+        <f aca="false">ROUND(F32*0.0025,0)*D32</f>
+        <v>0</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="K32" s="3" t="n">
         <v>8</v>
@@ -5492,7 +5473,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>114</v>
@@ -5504,18 +5485,23 @@
         <v>1</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="3" t="n">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="G33" s="3" t="n">
-        <f aca="false">ROUND(F33*0.0025,0)*D33</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J33" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="K33" s="3" t="n">
         <v>8</v>
       </c>
@@ -5530,10 +5516,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>115</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -5546,10 +5532,9 @@
         <v>1</v>
       </c>
       <c r="F34" s="3" t="n">
-        <v>93</v>
+        <v>986</v>
       </c>
       <c r="G34" s="3" t="n">
-        <f aca="false">ROUND(F34*0.0025,0)*D34</f>
         <v>0</v>
       </c>
       <c r="I34" s="3" t="s">
@@ -5570,10 +5555,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>83</v>
@@ -5585,20 +5570,15 @@
         <v>0</v>
       </c>
       <c r="F35" s="3" t="n">
-        <v>171</v>
+        <v>84</v>
       </c>
       <c r="G35" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>50</v>
+        <f aca="false">ROUND(F35*0.0025,0)*D35</f>
+        <v>0</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="K35" s="3" t="n">
         <v>8</v>
       </c>
@@ -5613,11 +5593,11 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>117</v>
+      <c r="A36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>83</v>
@@ -5629,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="n">
-        <v>986</v>
+        <v>313</v>
       </c>
       <c r="G36" s="3" t="n">
         <v>0</v>
@@ -5652,10 +5632,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>83</v>
@@ -5664,17 +5644,23 @@
         <v>1</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3" t="n">
-        <v>84</v>
+        <v>401</v>
       </c>
       <c r="G37" s="3" t="n">
         <f aca="false">ROUND(F37*0.0025,0)*D37</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="K37" s="3" t="n">
         <v>8</v>
@@ -5691,7 +5677,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>118</v>
@@ -5700,15 +5686,16 @@
         <v>83</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F38" s="3" t="n">
-        <v>313</v>
+        <v>119</v>
       </c>
       <c r="G38" s="3" t="n">
+        <f aca="false">ROUND(F38*0.0025,0)*D38</f>
         <v>0</v>
       </c>
       <c r="I38" s="3" t="s">
@@ -5729,13 +5716,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>83</v>
+        <v>120</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D39" s="3" t="n">
         <v>1</v>
@@ -5744,20 +5731,19 @@
         <v>1</v>
       </c>
       <c r="F39" s="3" t="n">
-        <v>401</v>
+        <v>1</v>
       </c>
       <c r="G39" s="3" t="n">
-        <f aca="false">ROUND(F39*0.0025,0)*D39</f>
         <v>1</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K39" s="3" t="n">
         <v>8</v>
@@ -5774,29 +5760,34 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>83</v>
+        <v>123</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="3" t="n">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="G40" s="3" t="n">
-        <f aca="false">ROUND(F40*0.0025,0)*D40</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>11</v>
+        <v>70</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="K40" s="3" t="n">
         <v>8</v>
@@ -5812,34 +5803,34 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" s="3" t="s">
+      <c r="F41" s="4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="J41" s="4" t="s">
         <v>71</v>
       </c>
       <c r="K41" s="3" t="n">
@@ -5856,35 +5847,35 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="3" t="n">
+        <v>121</v>
+      </c>
+      <c r="D42" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E42" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I42" s="3" t="s">
+      <c r="F42" s="4" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="J42" s="3" t="s">
-        <v>78</v>
+      <c r="J42" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="K42" s="3" t="n">
         <v>8</v>

</xml_diff>